<commit_message>
added tests for merged cells in excel
Signed-off-by: Peter Staar <taa@zurich.ibm.com>
</commit_message>
<xml_diff>
--- a/tests/data/xlsx/test-01.xlsx
+++ b/tests/data/xlsx/test-01.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taa/Documents/projects/docling/tests/data/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taa/Documents/projects/docling/tests/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58633F96-9EC5-AE4E-8AD9-B0D65C530CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84F6550-E88D-B54E-852B-F97BDC2CA6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{7BFEBC09-E794-024E-92A5-4E4755531B02}"/>
+    <workbookView xWindow="6520" yWindow="4900" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{7BFEBC09-E794-024E-92A5-4E4755531B02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t xml:space="preserve">first </t>
   </si>
@@ -58,6 +59,15 @@
   </si>
   <si>
     <t>col-4</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>header (f)</t>
+  </si>
+  <si>
+    <t>first (f)</t>
   </si>
 </sst>
 </file>
@@ -93,8 +103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2740,7 +2753,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2831,7 +2844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658ABF38-A604-D44B-9FDC-D737B2953C41}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
@@ -3067,4 +3080,157 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC60911-27E8-3D4F-B8AE-11B52351794B}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="1"/>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="1"/>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:G7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: added extraction of byte-images in excel (#804)
* fix(msexcel): ignore Mypy checking for _find_images_in_sheet function

Signed-off-by: Jiun An Tsai <andrew@247365-Macbook.local>

* fixed some issues

Signed-off-by: Peter Staar <taa@zurich.ibm.com>

* reformatted the code

Signed-off-by: Peter Staar <taa@zurich.ibm.com>

* pinned pillow in pyproject

Signed-off-by: Peter Staar <taa@zurich.ibm.com>

---------

Signed-off-by: Jiun An Tsai <andrew@247365-Macbook.local>
Signed-off-by: Peter Staar <taa@zurich.ibm.com>
Signed-off-by: Michele Dolfi <dol@zurich.ibm.com>
Co-authored-by: Jiun An Tsai <andrew@247365-Macbook.local>
Co-authored-by: Michele Dolfi <dol@zurich.ibm.com>
</commit_message>
<xml_diff>
--- a/tests/data/xlsx/test-01.xlsx
+++ b/tests/data/xlsx/test-01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taa/Documents/projects/docling/tests/data/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taa/Documents/projects/tmp/docling/tests/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84F6550-E88D-B54E-852B-F97BDC2CA6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945BD0F7-0ADB-A64A-9800-FEAA0742FEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="4900" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{7BFEBC09-E794-024E-92A5-4E4755531B02}"/>
+    <workbookView xWindow="12660" yWindow="-19220" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{7BFEBC09-E794-024E-92A5-4E4755531B02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2433,6 +2433,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>162530</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAC53083-F9CE-6543-CEEF-483A9D1A5B16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6766530" y="3784600"/>
+          <a:ext cx="3444270" cy="3517900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3232,5 +3281,6 @@
     <mergeCell ref="F7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>